<commit_message>
Pre-test per più zone coperte
</commit_message>
<xml_diff>
--- a/PS-VRP/INPUT_TEST/VEICOLI5.xlsx
+++ b/PS-VRP/INPUT_TEST/VEICOLI5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81037a9b1801ac22/Desktop/PS-VRP/Dati_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wikipedis\Documents\GitHub\progettoIS\PS-VRP\INPUT_TEST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{BCE6802B-3942-47BF-922B-ABBF4C8E4352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C8D1C65-DC44-4106-B222-9D0075D52C1F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BD9FA6-3029-48F0-88BA-097CE8412572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BA5BC94F-5D6C-4899-9888-A4EA67F19BD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -60,10 +60,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h\.mm;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,21 +95,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -118,12 +123,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -439,147 +440,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349B6A65-C9F6-4DE0-AA68-1A6BA01F8F97}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
         <v>45292</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
         <v>10000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>45292</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>10000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>45292</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
         <v>6000</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>45292</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
         <v>10000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>45293</v>
       </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
         <v>8000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>